<commit_message>
updated R002 in traceability matrix
</commit_message>
<xml_diff>
--- a/Documents/Testing/Tests Documents/traceability-matrix-template.xlsx
+++ b/Documents/Testing/Tests Documents/traceability-matrix-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Semeter_2\SFT\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/84e5bdbfc05febe3/Documents/CPASemester2/SFT221/SFT Project/winter24--sft221-naa-1/Documents/Testing/Tests Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB5AEEF-1E80-4D5E-B337-E8F4A238D631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{CFB5AEEF-1E80-4D5E-B337-E8F4A238D631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24B4AF2E-7CE4-4C68-802E-C00983D6D959}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{2BF2C2EA-6658-4885-BCA1-B03AABC6ADA8}"/>
+    <workbookView xWindow="4296" yWindow="1104" windowWidth="17196" windowHeight="10188" activeTab="2" xr2:uid="{2BF2C2EA-6658-4885-BCA1-B03AABC6ADA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="90">
   <si>
     <t>Requirements Traceability Matrix</t>
   </si>
@@ -175,9 +175,6 @@
     <t>Blackbox</t>
   </si>
   <si>
-    <t xml:space="preserve">FUNCTION: </t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -263,6 +260,57 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>FUNCTION: getInput</t>
+  </si>
+  <si>
+    <t>valid exit condition</t>
+  </si>
+  <si>
+    <t>Invalid exit condition</t>
+  </si>
+  <si>
+    <t>exit string</t>
+  </si>
+  <si>
+    <t>0 0 x</t>
+  </si>
+  <si>
+    <t>20.528x</t>
+  </si>
+  <si>
+    <t>No space delemited input</t>
+  </si>
+  <si>
+    <t>20 .5 28x</t>
+  </si>
+  <si>
+    <t>valid user input, space delimited</t>
+  </si>
+  <si>
+    <t>20   .5  28x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       20 .5 28x</t>
+  </si>
+  <si>
+    <t>Invalid, there should be no leading whitespace</t>
+  </si>
+  <si>
+    <t>Leading whitespace case</t>
+  </si>
+  <si>
+    <t>multiple space delimiter</t>
+  </si>
+  <si>
+    <t>Space delimited values</t>
+  </si>
+  <si>
+    <t>invalid, program needs separate values</t>
+  </si>
+  <si>
+    <t>Invalid user input, only one space delimiter per input</t>
   </si>
 </sst>
 </file>
@@ -316,7 +364,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -422,11 +470,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -450,6 +507,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -474,38 +538,44 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,6 +592,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -823,36 +897,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB4E6E5-98C4-49DD-9D54-D4CB0290F4DE}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.59765625" customWidth="1"/>
-    <col min="2" max="2" width="10.796875" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A2" s="12"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
       <c r="B2" s="1"/>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -879,15 +953,15 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -899,13 +973,13 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A4" s="14"/>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="19"/>
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -917,13 +991,13 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A5" s="14"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="19"/>
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -935,13 +1009,13 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A6" s="14"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="19"/>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -953,13 +1027,13 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A7" s="14"/>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="19"/>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -971,13 +1045,13 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A8" s="14"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="19"/>
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -989,13 +1063,13 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A9" s="14"/>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="19"/>
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -1007,13 +1081,13 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A10" s="14"/>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="19"/>
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1025,13 +1099,13 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A11" s="14"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="19"/>
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1043,13 +1117,15 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A12" s="14"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="19"/>
       <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1059,13 +1135,15 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A13" s="14"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
       <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1075,13 +1153,15 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A14" s="14"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
       <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1091,13 +1171,15 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A15" s="14"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="19"/>
       <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -1107,13 +1189,15 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A16" s="14"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="19"/>
       <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -1123,13 +1207,15 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A17" s="14"/>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="19"/>
       <c r="B17" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1139,8 +1225,8 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A18" s="14"/>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="19"/>
       <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
@@ -1155,8 +1241,8 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A19" s="14"/>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="19"/>
       <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
@@ -1171,8 +1257,8 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A20" s="14"/>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="19"/>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1187,8 +1273,8 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A21" s="14"/>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="19"/>
       <c r="B21" s="2" t="s">
         <v>28</v>
       </c>
@@ -1203,8 +1289,8 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A22" s="14"/>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="19"/>
       <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
@@ -1219,8 +1305,8 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A23" s="14"/>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="19"/>
       <c r="B23" s="2" t="s">
         <v>30</v>
       </c>
@@ -1235,8 +1321,8 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A24" s="14"/>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="19"/>
       <c r="B24" s="2" t="s">
         <v>31</v>
       </c>
@@ -1251,8 +1337,8 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A25" s="14"/>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="19"/>
       <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
@@ -1267,8 +1353,8 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A26" s="14"/>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="19"/>
       <c r="B26" s="2" t="s">
         <v>33</v>
       </c>
@@ -1283,10 +1369,10 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A27" s="14"/>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="19"/>
       <c r="B27" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1299,10 +1385,10 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A28" s="14"/>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="19"/>
       <c r="B28" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1315,10 +1401,10 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A29" s="14"/>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="19"/>
       <c r="B29" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1331,10 +1417,10 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A30" s="14"/>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="19"/>
       <c r="B30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1347,10 +1433,10 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A31" s="14"/>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="19"/>
       <c r="B31" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1379,60 +1465,60 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.9296875" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="18.46484375" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="17"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="18" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="29" t="s">
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="29" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="28"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="30"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -1440,19 +1526,19 @@
         <v>43</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1460,19 +1546,19 @@
         <v>43</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
@@ -1480,19 +1566,19 @@
         <v>43</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -1500,19 +1586,19 @@
         <v>43</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
@@ -1520,19 +1606,19 @@
         <v>43</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
@@ -1540,19 +1626,19 @@
         <v>43</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
@@ -1560,19 +1646,19 @@
         <v>43</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
@@ -1580,19 +1666,19 @@
         <v>43</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>17</v>
       </c>
@@ -1600,54 +1686,54 @@
         <v>43</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="31">
+        <v>58</v>
+      </c>
+      <c r="D12" s="14">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="10"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G24" s="8"/>
     </row>
   </sheetData>
@@ -1669,171 +1755,249 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C02FA876-2424-48F8-8D5E-D1F6D849256B}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="17"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="18"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C4" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C5" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C6" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="32"/>
+      <c r="E6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="7"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="7"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C7" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="32"/>
+      <c r="E7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="32"/>
+      <c r="E8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="32"/>
+      <c r="E9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="9"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" s="10"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="10"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G24" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="13">
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
+    <mergeCell ref="C3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1844,44 +2008,44 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="17"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="18" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="6" t="s">
         <v>40</v>
       </c>
@@ -1891,10 +2055,10 @@
       <c r="E3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="18"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F3" s="33"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" t="s">
         <v>43</v>
@@ -1903,7 +2067,7 @@
       <c r="D4" s="5"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" t="s">
         <v>43</v>
@@ -1912,7 +2076,7 @@
       <c r="D5" s="5"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" t="s">
         <v>43</v>
@@ -1921,7 +2085,7 @@
       <c r="D6" s="5"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" t="s">
         <v>43</v>
@@ -1930,66 +2094,66 @@
       <c r="D7" s="5"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="9"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" s="10"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="10"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G24" s="8"/>
     </row>
   </sheetData>
@@ -2013,41 +2177,41 @@
       <selection activeCell="A4" sqref="A4:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="17"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="18" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="6" t="s">
         <v>40</v>
       </c>
@@ -2057,10 +2221,10 @@
       <c r="E3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="18"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F3" s="33"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" t="s">
         <v>43</v>
@@ -2069,7 +2233,7 @@
       <c r="D4" s="5"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" t="s">
         <v>43</v>
@@ -2078,7 +2242,7 @@
       <c r="D5" s="5"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" t="s">
         <v>43</v>
@@ -2087,7 +2251,7 @@
       <c r="D6" s="5"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" t="s">
         <v>43</v>
@@ -2096,66 +2260,66 @@
       <c r="D7" s="5"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="9"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" s="10"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="10"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G24" s="8"/>
     </row>
   </sheetData>
@@ -2179,41 +2343,41 @@
       <selection activeCell="A4" sqref="A4:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="17"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="18" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="6" t="s">
         <v>40</v>
       </c>
@@ -2223,10 +2387,10 @@
       <c r="E3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="18"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F3" s="33"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" t="s">
         <v>43</v>
@@ -2235,7 +2399,7 @@
       <c r="D4" s="5"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" t="s">
         <v>43</v>
@@ -2244,7 +2408,7 @@
       <c r="D5" s="5"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" t="s">
         <v>43</v>
@@ -2253,7 +2417,7 @@
       <c r="D6" s="5"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" t="s">
         <v>43</v>
@@ -2262,66 +2426,66 @@
       <c r="D7" s="5"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="9"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" s="10"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="10"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G24" s="8"/>
     </row>
   </sheetData>
@@ -2345,41 +2509,41 @@
       <selection activeCell="A4" sqref="A4:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="17"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="18" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="6" t="s">
         <v>40</v>
       </c>
@@ -2389,10 +2553,10 @@
       <c r="E3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="18"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F3" s="33"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" t="s">
         <v>43</v>
@@ -2401,7 +2565,7 @@
       <c r="D4" s="5"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" t="s">
         <v>43</v>
@@ -2410,7 +2574,7 @@
       <c r="D5" s="5"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" t="s">
         <v>43</v>
@@ -2419,7 +2583,7 @@
       <c r="D6" s="5"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" t="s">
         <v>43</v>
@@ -2428,66 +2592,66 @@
       <c r="D7" s="5"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="9"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" s="10"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="10"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G24" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated functions.h, tracebility matrix and scrum report
</commit_message>
<xml_diff>
--- a/Documents/Testing/Tests Documents/traceability-matrix-template.xlsx
+++ b/Documents/Testing/Tests Documents/traceability-matrix-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jashandeep/Documents/GitHub/winter24--sft221-naa-1/Documents/Testing/Tests Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sft project\winter24--sft221-naa-1\Documents\Testing\Tests Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D1A85D-C3C1-A94A-A2EB-6B91024DB7E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEDCC1E-F4DB-4E82-AAE0-C6074A4BB97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="29400" windowHeight="17100" activeTab="7" xr2:uid="{2BF2C2EA-6658-4885-BCA1-B03AABC6ADA8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2BF2C2EA-6658-4885-BCA1-B03AABC6ADA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="149">
   <si>
     <t>Requirements Traceability Matrix</t>
   </si>
@@ -449,13 +449,52 @@
   </si>
   <si>
     <t>(X1=0,Y1=0),(X2=25,Y2=25)</t>
+  </si>
+  <si>
+    <t>Weight = 1 kg</t>
+  </si>
+  <si>
+    <t>Weight = 1000 kg, Truck current weight = 200 kg</t>
+  </si>
+  <si>
+    <t>The maximum valid weight that can be added to a truck with enough capacity.</t>
+  </si>
+  <si>
+    <t>Weight = 1001 kg</t>
+  </si>
+  <si>
+    <t>Weight over the maximum valid package weight.</t>
+  </si>
+  <si>
+    <t>Weight = 500 kg, Truck current weight = 800 kg</t>
+  </si>
+  <si>
+    <t>Truck would go over maximum capacity with the addition of the new package.</t>
+  </si>
+  <si>
+    <t>Weight = 300 kg, Truck current weight = 900 kg</t>
+  </si>
+  <si>
+    <t>Truck exactly at maximum capacity with the addition of the new package.</t>
+  </si>
+  <si>
+    <t>The minimum valid weight for a package.</t>
+  </si>
+  <si>
+    <t>Weight = 0 kg</t>
+  </si>
+  <si>
+    <t>Invalid weight for a package.</t>
+  </si>
+  <si>
+    <t>l</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -483,8 +522,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.6"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,8 +566,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -673,11 +730,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE3E3E3"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFE3E3E3"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE3E3E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE3E3E3"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE3E3E3"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFE3E3E3"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE3E3E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE3E3E3"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFE3E3E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE3E3E3"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE3E3E3"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFE3E3E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -708,87 +817,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -799,6 +827,99 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -818,9 +939,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -858,7 +979,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -964,7 +1085,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1106,7 +1227,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1116,36 +1237,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB4E6E5-98C4-49DD-9D54-D4CB0290F4DE}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="22"/>
       <c r="B2" s="1"/>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -1172,8 +1293,8 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1192,8 +1313,8 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="24"/>
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1210,8 +1331,8 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="24"/>
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1228,8 +1349,8 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="24"/>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
@@ -1246,8 +1367,8 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="24"/>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1264,8 +1385,8 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="24"/>
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1282,8 +1403,8 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="24"/>
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1300,8 +1421,8 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="24"/>
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1318,8 +1439,8 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="24"/>
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1336,8 +1457,8 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="24"/>
       <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1354,8 +1475,8 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="19"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="24"/>
       <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1372,8 +1493,8 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
       <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
@@ -1390,8 +1511,8 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="24"/>
       <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1408,8 +1529,8 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="24"/>
       <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1426,8 +1547,8 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="24"/>
       <c r="B17" s="2" t="s">
         <v>24</v>
       </c>
@@ -1444,8 +1565,8 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="24"/>
       <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
@@ -1462,8 +1583,8 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="24"/>
       <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
@@ -1480,8 +1601,8 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="24"/>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1498,8 +1619,8 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="19"/>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="24"/>
       <c r="B21" s="2" t="s">
         <v>28</v>
       </c>
@@ -1516,8 +1637,8 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="19"/>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="24"/>
       <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
@@ -1534,15 +1655,17 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="24"/>
       <c r="B23" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -1550,15 +1673,17 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="19"/>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="24"/>
       <c r="B24" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -1566,15 +1691,17 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="19"/>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="24"/>
       <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="F25" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -1582,15 +1709,17 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="19"/>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="24"/>
       <c r="B26" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="F26" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -1598,15 +1727,17 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="19"/>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="24"/>
       <c r="B27" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="F27" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -1614,15 +1745,17 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="19"/>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="24"/>
       <c r="B28" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
@@ -1630,8 +1763,8 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="19"/>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="24"/>
       <c r="B29" s="2" t="s">
         <v>69</v>
       </c>
@@ -1646,8 +1779,8 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="19"/>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="24"/>
       <c r="B30" s="2" t="s">
         <v>70</v>
       </c>
@@ -1662,8 +1795,8 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="19"/>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="24"/>
       <c r="B31" s="2" t="s">
         <v>71</v>
       </c>
@@ -1697,57 +1830,57 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="11" t="s">
         <v>44</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="13"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="30"/>
-    </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F3" s="33"/>
+      <c r="G3" s="35"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -1767,7 +1900,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1787,7 +1920,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
@@ -1807,7 +1940,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -1827,7 +1960,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
@@ -1847,7 +1980,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
@@ -1867,7 +2000,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
@@ -1887,7 +2020,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
@@ -1907,7 +2040,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>17</v>
       </c>
@@ -1927,42 +2060,42 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="10"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G24" s="8"/>
     </row>
   </sheetData>
@@ -1988,65 +2121,65 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" customWidth="1"/>
     <col min="7" max="7" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="32" t="s">
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="28" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="24" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="23"/>
-    </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="D3" s="40"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="28"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="15" t="s">
         <v>77</v>
       </c>
@@ -2057,17 +2190,17 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="35"/>
+      <c r="D5" s="36"/>
       <c r="E5" s="15" t="s">
         <v>72</v>
       </c>
@@ -2078,17 +2211,17 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="35"/>
+      <c r="D6" s="36"/>
       <c r="E6" t="s">
         <v>78</v>
       </c>
@@ -2099,17 +2232,17 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="35"/>
+      <c r="D7" s="36"/>
       <c r="E7" t="s">
         <v>80</v>
       </c>
@@ -2120,17 +2253,17 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="36"/>
       <c r="E8" t="s">
         <v>82</v>
       </c>
@@ -2141,17 +2274,17 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B9" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="D9" s="35"/>
+      <c r="D9" s="36"/>
       <c r="E9" t="s">
         <v>83</v>
       </c>
@@ -2162,64 +2295,58 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="9"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" s="10"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="10"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G24" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -2227,6 +2354,12 @@
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2237,44 +2370,44 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A1:G10"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="32" t="s">
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="28" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="6" t="s">
         <v>40</v>
       </c>
@@ -2284,10 +2417,10 @@
       <c r="E3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="23"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="38"/>
+      <c r="G3" s="28"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>16</v>
       </c>
@@ -2310,7 +2443,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>17</v>
       </c>
@@ -2333,7 +2466,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>18</v>
       </c>
@@ -2356,7 +2489,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>19</v>
       </c>
@@ -2379,7 +2512,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>20</v>
       </c>
@@ -2402,60 +2535,60 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="9"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" s="10"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="10"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G24" s="8"/>
     </row>
   </sheetData>
@@ -2476,164 +2609,220 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
+    </row>
+    <row r="2" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="D2" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>39</v>
+      </c>
       <c r="F2" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="23"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+        <v>148</v>
+      </c>
+      <c r="G2" s="34"/>
+    </row>
+    <row r="3" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="33"/>
+      <c r="G3" s="35"/>
+    </row>
+    <row r="4" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>138</v>
+      </c>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+    <row r="5" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="51" t="s">
+        <v>140</v>
+      </c>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+    <row r="6" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="51" t="s">
+        <v>142</v>
+      </c>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+    <row r="7" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="51" t="s">
+        <v>144</v>
+      </c>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>147</v>
+      </c>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="9"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" s="10"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="10"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G24" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2645,47 +2834,47 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="30"/>
-    </row>
-    <row r="4" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+      <c r="D3" s="33"/>
+      <c r="E3" s="35"/>
+    </row>
+    <row r="4" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -2702,7 +2891,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -2719,7 +2908,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -2736,7 +2925,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" t="s">
         <v>43</v>
@@ -2751,61 +2940,61 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="C8" s="5"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="C9" s="5"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="C10" s="5"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E24" s="8"/>
     </row>
   </sheetData>
@@ -2828,62 +3017,62 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.83203125" customWidth="1"/>
-    <col min="7" max="7" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.77734375" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="32" t="s">
+      <c r="D2" s="43"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="28" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="23"/>
-    </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="28"/>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
       <c r="F4" t="s">
         <v>92</v>
       </c>
@@ -2891,16 +3080,16 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
       <c r="F5" t="s">
         <v>92</v>
       </c>
@@ -2908,16 +3097,16 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
       <c r="F6" t="s">
         <v>92</v>
       </c>
@@ -2925,16 +3114,16 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
       <c r="F7" t="s">
         <v>92</v>
       </c>
@@ -2942,16 +3131,16 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
       <c r="F8" t="s">
         <v>59</v>
       </c>
@@ -2959,75 +3148,75 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="9"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" s="10"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="10"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G24" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3038,162 +3227,162 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA7D5DB-916A-BB49-823D-FF2F3FE56BCF}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="D12" zoomScale="92" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" customWidth="1"/>
     <col min="4" max="4" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="28" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="23"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="43"/>
-      <c r="B4" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="45" t="s">
+      <c r="D3" s="38"/>
+      <c r="E3" s="28"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="43"/>
-      <c r="B5" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="45" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="19">
         <v>6.7</v>
       </c>
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="43"/>
-      <c r="B6" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="45" t="s">
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="44">
+      <c r="D6" s="17">
         <v>0</v>
       </c>
-      <c r="E6" s="44" t="s">
+      <c r="E6" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="43"/>
-      <c r="B7" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="45" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="43"/>
-      <c r="B8" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="45" t="s">
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="16"/>
+      <c r="B8" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="19">
         <v>35.35</v>
       </c>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="43"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="43"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="44"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
update Final Test Report
</commit_message>
<xml_diff>
--- a/Documents/Testing/Tests Documents/traceability-matrix-template.xlsx
+++ b/Documents/Testing/Tests Documents/traceability-matrix-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Semeter_2\SFT\MS4\Documents\Testing\Tests Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Semeter_2\SFT\Final\Documents\Testing\Tests Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE9B528-4B8D-432D-80BD-E99D83EC64AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFD5EE8-7141-49E1-9861-93130F7D5CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{2BF2C2EA-6658-4885-BCA1-B03AABC6ADA8}"/>
   </bookViews>
@@ -352,7 +352,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,12 +386,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -454,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -478,8 +472,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB4E6E5-98C4-49DD-9D54-D4CB0290F4DE}">
   <dimension ref="A1:P91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="83" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44:G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1317,7 +1309,7 @@
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F26" s="3"/>
@@ -1335,7 +1327,7 @@
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F27" s="3"/>
@@ -1426,7 +1418,7 @@
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="13" t="s">
+      <c r="F32" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G32" s="3"/>
@@ -1444,7 +1436,7 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="13" t="s">
+      <c r="F33" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G33" s="3"/>
@@ -1661,7 +1653,7 @@
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="13" t="s">
+      <c r="G45" s="6" t="s">
         <v>39</v>
       </c>
       <c r="H45" s="3"/>
@@ -1679,7 +1671,7 @@
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="14" t="s">
+      <c r="G46" s="6" t="s">
         <v>39</v>
       </c>
       <c r="H46" s="3"/>

</xml_diff>

<commit_message>
remove r06 r07 from matrix
</commit_message>
<xml_diff>
--- a/Documents/Testing/Tests Documents/traceability-matrix-template.xlsx
+++ b/Documents/Testing/Tests Documents/traceability-matrix-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Semeter_2\SFT\Final\Documents\Testing\Tests Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPASemester2\SFT221\SFT Project\winter24--sft221-naa-1\Documents\Testing\Tests Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFD5EE8-7141-49E1-9861-93130F7D5CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699051AB-A60F-43FA-B9D1-1407DE13600C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{2BF2C2EA-6658-4885-BCA1-B03AABC6ADA8}"/>
+    <workbookView xWindow="2184" yWindow="576" windowWidth="20856" windowHeight="11664" xr2:uid="{2BF2C2EA-6658-4885-BCA1-B03AABC6ADA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="95">
   <si>
     <t>Requirements Traceability Matrix</t>
   </si>
@@ -57,12 +57,6 @@
     <t>R005</t>
   </si>
   <si>
-    <t>R006</t>
-  </si>
-  <si>
-    <t>R007</t>
-  </si>
-  <si>
     <t>T001</t>
   </si>
   <si>
@@ -265,12 +259,6 @@
   </si>
   <si>
     <t>Truck have enough to space to have 50 cubic meter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add route to map </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distance of starting point and delivery </t>
   </si>
   <si>
     <t>User input correct requirement</t>
@@ -352,7 +340,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,12 +368,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -456,7 +438,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -786,38 +767,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB4E6E5-98C4-49DD-9D54-D4CB0290F4DE}">
-  <dimension ref="A1:P91"/>
+  <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44:G46"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="83" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.453125" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
       <c r="B2" s="1"/>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -834,25 +813,19 @@
       <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -861,16 +834,14 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="9"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -879,16 +850,14 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="9"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -897,16 +866,14 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -915,16 +882,14 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="9"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -933,16 +898,14 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -951,16 +914,14 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="9"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="8"/>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -969,22 +930,20 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="O9" t="s">
+      <c r="M9" t="s">
+        <v>71</v>
+      </c>
+      <c r="N9" t="s">
         <v>73</v>
       </c>
-      <c r="P9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -993,22 +952,20 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="O10" t="s">
+      <c r="M10" t="s">
         <v>3</v>
       </c>
-      <c r="P10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
+      <c r="N10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="8"/>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1017,23 +974,21 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="O11" t="s">
+      <c r="M11" t="s">
         <v>4</v>
       </c>
-      <c r="P11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="9"/>
+      <c r="N11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="8"/>
       <c r="B12" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1041,23 +996,21 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="O12" t="s">
+      <c r="M12" t="s">
         <v>5</v>
       </c>
-      <c r="P12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" s="9"/>
+      <c r="N12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
       <c r="B13" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1065,23 +1018,21 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="O13" t="s">
+      <c r="M13" t="s">
         <v>6</v>
       </c>
-      <c r="P13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" s="9"/>
+      <c r="N13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="8"/>
       <c r="B14" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1089,23 +1040,15 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="O14" t="s">
-        <v>7</v>
-      </c>
-      <c r="P14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A15" s="9"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="8"/>
       <c r="B15" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -1113,23 +1056,15 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="O15" t="s">
-        <v>8</v>
-      </c>
-      <c r="P15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="8"/>
       <c r="B16" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1137,17 +1072,15 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A17" s="9"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="8"/>
       <c r="B17" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -1155,17 +1088,15 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="9"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="8"/>
       <c r="B18" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -1173,17 +1104,15 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" s="9"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="8"/>
       <c r="B19" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -1191,17 +1120,15 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" s="9"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="8"/>
       <c r="B20" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1209,643 +1136,553 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" s="9"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="8"/>
       <c r="B21" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" s="9"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="8"/>
       <c r="B22" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" s="9"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="8"/>
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24" s="9"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="8"/>
       <c r="B24" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A25" s="9"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="8"/>
       <c r="B25" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="8"/>
       <c r="B26" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A27" s="9"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="8"/>
       <c r="B27" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A28" s="9"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="8"/>
       <c r="B28" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A29" s="9"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="8"/>
       <c r="B29" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A30" s="9"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="8"/>
       <c r="B30" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A31" s="9"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="8"/>
       <c r="B31" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A32" s="9"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="8"/>
       <c r="B32" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A33" s="9"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="8"/>
       <c r="B33" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-    </row>
-    <row r="34" spans="1:12" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="9"/>
+    </row>
+    <row r="34" spans="1:10" ht="18.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="8"/>
       <c r="B34" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-    </row>
-    <row r="35" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="9"/>
+    </row>
+    <row r="35" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="8"/>
       <c r="B35" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A36" s="9"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="8"/>
       <c r="B36" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A37" s="9"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="8"/>
       <c r="B37" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A38" s="9"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="8"/>
       <c r="B38" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A39" s="9"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="8"/>
       <c r="B39" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A40" s="9"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="8"/>
       <c r="B40" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A41" s="9"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="8"/>
       <c r="B41" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A42" s="9"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="8"/>
       <c r="B42" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A43" s="9"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="8"/>
       <c r="B43" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A44" s="9"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="8"/>
       <c r="B44" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A45" s="9"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="8"/>
       <c r="B45" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A46" s="9"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="8"/>
       <c r="B46" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A47" s="9"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="8"/>
       <c r="B47" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
-      <c r="H47" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A48" s="9"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="8"/>
       <c r="B48" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
-      <c r="H48" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A49" s="9"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="8"/>
       <c r="B49" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
-      <c r="H49" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A50" s="9"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="8"/>
       <c r="B50" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
-      <c r="H50" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A51" s="9"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="8"/>
       <c r="B51" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
-      <c r="H51" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="H51" s="3"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A52" s="9"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="8"/>
       <c r="B52" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
-      <c r="H52" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A53" s="9"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="8"/>
       <c r="B53" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
-      <c r="H53" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A54" s="9"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="8"/>
       <c r="B54" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
-      <c r="H54" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
-      <c r="L54" s="3"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A55" s="9"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="8"/>
       <c r="B55" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
-      <c r="H55" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A56" s="9"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="8"/>
       <c r="B56" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -1853,17 +1690,13 @@
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
-      <c r="I56" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I56" s="3"/>
       <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
-      <c r="L56" s="3"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A57" s="9"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="8"/>
       <c r="B57" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -1871,17 +1704,13 @@
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
-      <c r="I57" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I57" s="3"/>
       <c r="J57" s="3"/>
-      <c r="K57" s="3"/>
-      <c r="L57" s="3"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A58" s="9"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="8"/>
       <c r="B58" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -1889,17 +1718,13 @@
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
-      <c r="I58" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I58" s="3"/>
       <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A59" s="9"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="8"/>
       <c r="B59" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -1907,17 +1732,13 @@
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
-      <c r="I59" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I59" s="3"/>
       <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
-      <c r="L59" s="3"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A60" s="9"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="8"/>
       <c r="B60" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -1925,17 +1746,13 @@
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
-      <c r="I60" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I60" s="3"/>
       <c r="J60" s="3"/>
-      <c r="K60" s="3"/>
-      <c r="L60" s="3"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A61" s="9"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" s="8"/>
       <c r="B61" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -1943,17 +1760,13 @@
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
-      <c r="I61" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I61" s="3"/>
       <c r="J61" s="3"/>
-      <c r="K61" s="3"/>
-      <c r="L61" s="3"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A62" s="12"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="11"/>
       <c r="B62" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -1961,17 +1774,13 @@
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
-      <c r="I62" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I62" s="3"/>
       <c r="J62" s="3"/>
-      <c r="K62" s="3"/>
-      <c r="L62" s="3"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A63" s="12"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="11"/>
       <c r="B63" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -1979,17 +1788,13 @@
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
-      <c r="I63" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I63" s="3"/>
       <c r="J63" s="3"/>
-      <c r="K63" s="3"/>
-      <c r="L63" s="3"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A64" s="12"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" s="11"/>
       <c r="B64" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -1997,17 +1802,13 @@
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
-      <c r="I64" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I64" s="3"/>
       <c r="J64" s="3"/>
-      <c r="K64" s="3"/>
-      <c r="L64" s="3"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A65" s="12"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" s="11"/>
       <c r="B65" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -2015,17 +1816,13 @@
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
-      <c r="I65" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I65" s="3"/>
       <c r="J65" s="3"/>
-      <c r="K65" s="3"/>
-      <c r="L65" s="3"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A66" s="12"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" s="11"/>
       <c r="B66" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -2033,17 +1830,13 @@
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
-      <c r="I66" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I66" s="3"/>
       <c r="J66" s="3"/>
-      <c r="K66" s="3"/>
-      <c r="L66" s="3"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A67" s="12"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" s="11"/>
       <c r="B67" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -2051,17 +1844,13 @@
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
-      <c r="I67" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I67" s="3"/>
       <c r="J67" s="3"/>
-      <c r="K67" s="3"/>
-      <c r="L67" s="3"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A68" s="12"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" s="11"/>
       <c r="B68" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -2069,17 +1858,13 @@
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
-      <c r="I68" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I68" s="3"/>
       <c r="J68" s="3"/>
-      <c r="K68" s="3"/>
-      <c r="L68" s="3"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A69" s="12"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="11"/>
       <c r="B69" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -2087,17 +1872,13 @@
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
-      <c r="I69" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I69" s="3"/>
       <c r="J69" s="3"/>
-      <c r="K69" s="3"/>
-      <c r="L69" s="3"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A70" s="12"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="11"/>
       <c r="B70" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -2105,17 +1886,13 @@
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
-      <c r="I70" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I70" s="3"/>
       <c r="J70" s="3"/>
-      <c r="K70" s="3"/>
-      <c r="L70" s="3"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A71" s="12"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" s="11"/>
       <c r="B71" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
@@ -2123,17 +1900,13 @@
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
-      <c r="I71" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I71" s="3"/>
       <c r="J71" s="3"/>
-      <c r="K71" s="3"/>
-      <c r="L71" s="3"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A72" s="12"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" s="11"/>
       <c r="B72" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
@@ -2141,17 +1914,13 @@
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
-      <c r="I72" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I72" s="3"/>
       <c r="J72" s="3"/>
-      <c r="K72" s="3"/>
-      <c r="L72" s="3"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A73" s="12"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" s="11"/>
       <c r="B73" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
@@ -2159,396 +1928,340 @@
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
-      <c r="I73" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="I73" s="3"/>
       <c r="J73" s="3"/>
-      <c r="K73" s="3"/>
-      <c r="L73" s="3"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A74" s="12"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" s="11"/>
       <c r="B74" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
-      <c r="I74" s="7"/>
+      <c r="I74" s="3"/>
       <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
-      <c r="L74" s="3"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A75" s="12"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" s="11"/>
       <c r="B75" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D75" s="3"/>
       <c r="E75" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
-      <c r="I75" s="7"/>
+      <c r="I75" s="3"/>
       <c r="J75" s="3"/>
-      <c r="K75" s="3"/>
-      <c r="L75" s="3"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A76" s="12"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="11"/>
       <c r="B76" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
-      <c r="I76" s="7"/>
+      <c r="I76" s="3"/>
       <c r="J76" s="3"/>
-      <c r="K76" s="3"/>
-      <c r="L76" s="3"/>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A77" s="12"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="11"/>
       <c r="B77" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
-      <c r="I77" s="7"/>
+      <c r="I77" s="3"/>
       <c r="J77" s="3"/>
-      <c r="K77" s="3"/>
-      <c r="L77" s="3"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A78" s="12"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="11"/>
       <c r="B78" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
-      <c r="I78" s="7"/>
+      <c r="I78" s="3"/>
       <c r="J78" s="3"/>
-      <c r="K78" s="3"/>
-      <c r="L78" s="3"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A79" s="12"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="11"/>
       <c r="B79" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
-      <c r="I79" s="7"/>
+      <c r="I79" s="3"/>
       <c r="J79" s="3"/>
-      <c r="K79" s="3"/>
-      <c r="L79" s="3"/>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A80" s="12"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="11"/>
       <c r="B80" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
       <c r="E80" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F80" s="3"/>
       <c r="G80" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H80" s="3"/>
-      <c r="I80" s="7"/>
+      <c r="I80" s="3"/>
       <c r="J80" s="3"/>
-      <c r="K80" s="3"/>
-      <c r="L80" s="3"/>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A81" s="12"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" s="11"/>
       <c r="B81" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="E81" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F81" s="3"/>
       <c r="G81" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H81" s="3"/>
-      <c r="I81" s="7"/>
+      <c r="I81" s="3"/>
       <c r="J81" s="3"/>
-      <c r="K81" s="3"/>
-      <c r="L81" s="3"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A82" s="12"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" s="11"/>
       <c r="B82" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
       <c r="E82" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F82" s="3"/>
       <c r="G82" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H82" s="3"/>
-      <c r="I82" s="7"/>
+      <c r="I82" s="3"/>
       <c r="J82" s="3"/>
-      <c r="K82" s="3"/>
-      <c r="L82" s="3"/>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A83" s="12"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" s="11"/>
       <c r="B83" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
       <c r="E83" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F83" s="3"/>
       <c r="G83" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H83" s="3"/>
-      <c r="I83" s="7"/>
+      <c r="I83" s="3"/>
       <c r="J83" s="3"/>
-      <c r="K83" s="3"/>
-      <c r="L83" s="3"/>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A84" s="12"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="11"/>
       <c r="B84" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E84" s="3"/>
       <c r="F84" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
-      <c r="I84" s="7"/>
+      <c r="I84" s="3"/>
       <c r="J84" s="3"/>
-      <c r="K84" s="3"/>
-      <c r="L84" s="3"/>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A85" s="12"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="11"/>
       <c r="B85" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E85" s="3"/>
       <c r="F85" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
-      <c r="I85" s="7"/>
+      <c r="I85" s="3"/>
       <c r="J85" s="3"/>
-      <c r="K85" s="3"/>
-      <c r="L85" s="3"/>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A86" s="12"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="11"/>
       <c r="B86" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E86" s="3"/>
       <c r="F86" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
-      <c r="I86" s="7"/>
+      <c r="I86" s="3"/>
       <c r="J86" s="3"/>
-      <c r="K86" s="3"/>
-      <c r="L86" s="3"/>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A87" s="12"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87" s="11"/>
       <c r="B87" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E87" s="3"/>
       <c r="F87" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
-      <c r="I87" s="7"/>
+      <c r="I87" s="3"/>
       <c r="J87" s="3"/>
-      <c r="K87" s="3"/>
-      <c r="L87" s="3"/>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A88" s="12"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" s="11"/>
       <c r="B88" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
-      <c r="H88" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I88" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="H88" s="3"/>
+      <c r="I88" s="3"/>
       <c r="J88" s="3"/>
-      <c r="K88" s="3"/>
-      <c r="L88" s="3"/>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A89" s="12"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A89" s="11"/>
       <c r="B89" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
-      <c r="H89" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I89" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="H89" s="3"/>
+      <c r="I89" s="3"/>
       <c r="J89" s="3"/>
-      <c r="K89" s="3"/>
-      <c r="L89" s="3"/>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A90" s="12"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90" s="11"/>
       <c r="B90" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
-      <c r="H90" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I90" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="H90" s="3"/>
+      <c r="I90" s="3"/>
       <c r="J90" s="3"/>
-      <c r="K90" s="3"/>
-      <c r="L90" s="3"/>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A91" s="12"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" s="11"/>
       <c r="B91" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
-      <c r="H91" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I91" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
       <c r="J91" s="3"/>
-      <c r="K91" s="3"/>
-      <c r="L91" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="C1:J1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A62:A91"/>
   </mergeCells>

</xml_diff>